<commit_message>
Dodani rezultati za citiranost UKCL in posodobljeni podatki
</commit_message>
<xml_diff>
--- a/data/publikacije.xlsx
+++ b/data/publikacije.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28957\Documents\DELO\prog_skupine_raz_uspesnost\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA2FC08-19E2-4197-91F1-2A1107F1F947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE08616C-7AE4-4B9C-AA5A-4B585B0AA93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E0CBE77D-3269-4022-B168-B59C194AE0FC}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="41472" windowHeight="16752" xr2:uid="{E0CBE77D-3269-4022-B168-B59C194AE0FC}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -420,7 +420,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +507,7 @@
         <v>2024</v>
       </c>
       <c r="B8">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c r="C8">
         <v>101</v>

</xml_diff>